<commit_message>
tidying up commit before handoff
</commit_message>
<xml_diff>
--- a/data/filename_to_sample.xlsx
+++ b/data/filename_to_sample.xlsx
@@ -190,7 +190,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -217,13 +217,25 @@
       <name val="ArialMT"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -235,7 +247,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -245,13 +257,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="9"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
+    <cellStyle name="Bad" xfId="9" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -575,7 +590,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -690,36 +705,36 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>3</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
         <v>2</v>
       </c>
     </row>
@@ -792,19 +807,19 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>3</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="3">
         <v>2</v>
       </c>
     </row>

</xml_diff>